<commit_message>
Updated invalid inputs sheet
</commit_message>
<xml_diff>
--- a/DataSheets/GetAgileProductGTIN_DataSheet.xlsx
+++ b/DataSheets/GetAgileProductGTIN_DataSheet.xlsx
@@ -95,9 +95,6 @@
     <t>PartNumber does not exist</t>
   </si>
   <si>
-    <t>AR-JUNK</t>
-  </si>
-  <si>
     <t>errorCode</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>wasSuccessful</t>
+  </si>
+  <si>
+    <t>AR-JUNK2</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,13 +690,13 @@
         <v>18</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -715,10 +715,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="6"/>
@@ -734,16 +734,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="4"/>

</xml_diff>